<commit_message>
changes: payment: remind kirim ke brand dan h-1 posting: remind h-1 dan optional all: batch gausah dibaca
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\900949\Desktop\ramu\Ramu Agency\Ramu Agency\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indocyber\Desktop\projects\ramu\UiPath\ramu-reminder\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4CE78F-26C3-4167-85CB-466E0B3C2CA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6FB9A1-ED20-4E2C-9173-43BD13F6301B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5556" xr2:uid="{360D7E17-4C01-43E3-9410-7F6DDD56814D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{360D7E17-4C01-43E3-9410-7F6DDD56814D}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -45,30 +45,25 @@
     <t>Reminder_Kol_Visit</t>
   </si>
   <si>
-    <t>*RECAP JADWAL PERMINGGU: Kak [KOL Name] dan Kesibukannya😭🫶🏻*
+    <t>Reminder_Kol_Payment</t>
+  </si>
+  <si>
+    <t>*RECAP JADWAL PERMINGGU from RAMU🫶🏻*
 Hi kak [KOL Name]! 
-Berhubung minggu ini kayaknya kakak cukup padat, Ramu coba bantu listing endorsement tasknya yaa! Kita coba urut dari yang paling urgent🤙🏻[Data]
+Selamat ya untuk project-project yang masuk di bulan ini. Untuk mempermudah schedule, Ramu coba bantu listing endorsement tasknya yaa! Aku coba urut dari yang paling urgent🤙🏻[Data]
 Semangaatt kak!!😭🫶🏻 Kalau ada something kabarin aku yaaakk</t>
   </si>
   <si>
-    <t>Approved: [Brand] Bisa Diposting😎🤙🏻
+    <t>*Approved: [Brand] Bisa Diposting😎🤙🏻*
 Hi kak [KOL]!
 Nice banget untuk draft kemarin sudah diapprove sesuai timeline. So, jangan lupaa ya besok masuk jadwal posting, ini detailnya:
 - SOW: [SOW]
 - ⁠Tanggal: [Posting]
-- ⁠Jam: 19:00 - 20:00 WIB
+- ⁠Jam: 19:00 - 20:00 maks
 Kalau udah dipost kabarin yaa kak🫶🏻</t>
   </si>
   <si>
-    <t>Gentle Reminder: H-1 Deadline⚠‼
-Hi kak …, apaa kabarr ni? Semoga selalu dalam keadaan well yahh😎🤙🏻 Btw kak punten, aku mau reminder kalau besok kita ada deadline drafting yaa! Ini detailnya:
-✨Brand: [Nama Brand]
-📝 Deadline: [Day, DD/MM/YYYY]
-👉🏻Storyline approved: [Link Storyline]
-Kalau ada kendala atau yang dibingungin sama briefnya kabarin aku yahh. Mohon bantuannya jangan sampai telat yaa kakk hihiw. Thankyou</t>
-  </si>
-  <si>
-    <t>BESOK VISIT: [Brand]✨
+    <t>*BESOK VISIT: [Brand]✨*
 Hi kak [KOL Name], ini reminder dari Ramu untuk infoin detail visit besok yaaa!
 🗓 Detail Visit
 - Tanggal: [Tanggal Visit]
@@ -88,12 +83,19 @@
 Thankyou so much yaaa kak! Semangat teruuss yaa. Kalau ada yang mau didiskusikan let us know yaaa🥰</t>
   </si>
   <si>
-    <t>Reminder_Kol_Payment</t>
-  </si>
-  <si>
-    <t>Nama Brand : [Brand]
+    <t>*Reminder Payment from RAMU*
+Hi kak [Nama PIC], semoga selalu dalam keadaan sehat ya. Punten aku izin follow up terkait payment project [Brand] dengan [KOL Name] yaaa. 
 Nominal : [Nominal]
-Tanggal : [Tanggal]</t>
+Tenggat : [Tanggal]
+Kalau semisal sudah ada bukti transfernya mohon kabari aku yaa kak. Thank you!</t>
+  </si>
+  <si>
+    <t>*Gentle Reminder: H-1 Deadline⚠‼*
+Hi kak [KOL], apaa kabar ni? Semoga selalu dalam keadaan well yahh😎🤙🏻 Btw kak punten, aku mau reminder kalau besok kita ada deadline drafting yaa! Ini detailnya:
+✨Brand: [Nama Brand]
+📝 Deadline: [Day, DD/MM/YYYY]
+👉🏻Storyline approved: [Link Storyline]
+Kalau ada kendala atau yang dibingungin sama briefnya kabarin aku yahh. Mohon bantuannya jangan sampai telat yaa kakk hihiw. Thankyou</t>
   </si>
 </sst>
 </file>
@@ -476,17 +478,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA5BC9A-9EA4-49DF-AE64-4CE35A3209DB}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="119" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
-    <col min="2" max="2" width="39.21875" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -494,31 +496,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="175.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="175" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="174" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="377" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -526,119 +528,119 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
     </row>

</xml_diff>